<commit_message>
updated excel plot for exp 4.1
</commit_message>
<xml_diff>
--- a/week1/experiments/exp3/Kai_Experiment_3_attempt_2.xlsx
+++ b/week1/experiments/exp3/Kai_Experiment_3_attempt_2.xlsx
@@ -989,11 +989,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119188096"/>
-        <c:axId val="119198464"/>
+        <c:axId val="118160000"/>
+        <c:axId val="118293248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119188096"/>
+        <c:axId val="118160000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1027,12 +1027,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119198464"/>
+        <c:crossAx val="118293248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119198464"/>
+        <c:axId val="118293248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1067,7 +1067,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119188096"/>
+        <c:crossAx val="118160000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2108,11 +2108,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119127424"/>
-        <c:axId val="119133696"/>
+        <c:axId val="118340992"/>
+        <c:axId val="118351360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119127424"/>
+        <c:axId val="118340992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2146,12 +2146,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119133696"/>
+        <c:crossAx val="118351360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119133696"/>
+        <c:axId val="118351360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2186,7 +2186,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119127424"/>
+        <c:crossAx val="118340992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3227,11 +3227,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119374592"/>
-        <c:axId val="119376512"/>
+        <c:axId val="118842112"/>
+        <c:axId val="118844032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119374592"/>
+        <c:axId val="118842112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3265,12 +3265,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119376512"/>
+        <c:crossAx val="118844032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119376512"/>
+        <c:axId val="118844032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3305,7 +3305,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119374592"/>
+        <c:crossAx val="118842112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4346,11 +4346,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="120927360"/>
-        <c:axId val="120929280"/>
+        <c:axId val="118891648"/>
+        <c:axId val="118893568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120927360"/>
+        <c:axId val="118891648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4384,12 +4384,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120929280"/>
+        <c:crossAx val="118893568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120929280"/>
+        <c:axId val="118893568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4424,7 +4424,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120927360"/>
+        <c:crossAx val="118891648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6672,7 +6672,7 @@
         <v>7</v>
       </c>
       <c r="T14" s="3">
-        <f t="shared" ref="T14:T28" si="12">R14*60+S14</f>
+        <f t="shared" ref="T14:T27" si="12">R14*60+S14</f>
         <v>367</v>
       </c>
       <c r="U14" s="3">
@@ -8674,7 +8674,7 @@
         <v>26</v>
       </c>
       <c r="T28" s="7">
-        <f>R28*60+S28</f>
+        <f t="shared" ref="T28:T36" si="17">R28*60+S28</f>
         <v>806</v>
       </c>
       <c r="U28" s="7">
@@ -8817,7 +8817,7 @@
         <v>58</v>
       </c>
       <c r="T29" s="5">
-        <f>R29*60+S29</f>
+        <f t="shared" si="17"/>
         <v>838</v>
       </c>
       <c r="U29" s="5">
@@ -8960,7 +8960,7 @@
         <v>56</v>
       </c>
       <c r="T30" s="5">
-        <f>R30*60+S30</f>
+        <f t="shared" si="17"/>
         <v>896</v>
       </c>
       <c r="U30" s="5">
@@ -9103,7 +9103,7 @@
         <v>21</v>
       </c>
       <c r="T31" s="5">
-        <f>R31*60+S31</f>
+        <f t="shared" si="17"/>
         <v>921</v>
       </c>
       <c r="U31" s="5">
@@ -9246,7 +9246,7 @@
         <v>52</v>
       </c>
       <c r="T32" s="5">
-        <f>R32*60+S32</f>
+        <f t="shared" si="17"/>
         <v>952</v>
       </c>
       <c r="U32" s="5">
@@ -9389,7 +9389,7 @@
         <v>16</v>
       </c>
       <c r="T33" s="5">
-        <f>R33*60+S33</f>
+        <f t="shared" si="17"/>
         <v>1276</v>
       </c>
       <c r="U33" s="5">
@@ -9532,7 +9532,7 @@
         <v>1</v>
       </c>
       <c r="T34" s="5">
-        <f>R34*60+S34</f>
+        <f t="shared" si="17"/>
         <v>1321</v>
       </c>
       <c r="U34" s="5">
@@ -9675,7 +9675,7 @@
         <v>22</v>
       </c>
       <c r="T35" s="5">
-        <f>R35*60+S35</f>
+        <f t="shared" si="17"/>
         <v>1702</v>
       </c>
       <c r="U35" s="5">
@@ -9818,7 +9818,7 @@
         <v>46</v>
       </c>
       <c r="T36" s="5">
-        <f>R36*60+S36</f>
+        <f t="shared" si="17"/>
         <v>1906</v>
       </c>
       <c r="U36" s="5">
@@ -9913,8 +9913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AM5" sqref="AM5"/>
+    <sheetView tabSelected="1" topLeftCell="P42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>